<commit_message>
Agregar manejo de excepciones al abrir y guardar archivos, mejorar validaciones y actualizar mensajes en la gestión de frutas
</commit_message>
<xml_diff>
--- a/inventario.xlsx
+++ b/inventario.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -445,7 +445,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C2" t="n">
         <v>1</v>
@@ -458,7 +458,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="C3" t="n">
         <v>0.6</v>
@@ -471,23 +471,10 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>4</v>
+        <v>33</v>
       </c>
       <c r="C4" t="n">
         <v>0.5</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Sandia</t>
-        </is>
-      </c>
-      <c r="B5" t="n">
-        <v>50</v>
-      </c>
-      <c r="C5" t="n">
-        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualizar archivo de inventario.xlsx con nuevos datos
</commit_message>
<xml_diff>
--- a/inventario.xlsx
+++ b/inventario.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -445,7 +445,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>33</v>
+        <v>66</v>
       </c>
       <c r="C2" t="n">
         <v>1</v>
@@ -475,6 +475,19 @@
       </c>
       <c r="C4" t="n">
         <v>0.5</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Cereza</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>33</v>
+      </c>
+      <c r="C5" t="n">
+        <v>1.1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>